<commit_message>
feat: Search using title from VBODA Database
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="43">
   <si>
     <t>Test</t>
   </si>
@@ -115,6 +115,39 @@
   </si>
   <si>
     <t>Tes</t>
+  </si>
+  <si>
+    <t>Holberg Suite</t>
+  </si>
+  <si>
+    <t>Edward Grieg</t>
+  </si>
+  <si>
+    <t>Mvmts 1, 3, 5 ONLY</t>
+  </si>
+  <si>
+    <t>Waltz No. 2</t>
+  </si>
+  <si>
+    <t>Shostakovich</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Cello solo!</t>
+  </si>
+  <si>
+    <t>Winter Melodies</t>
+  </si>
+  <si>
+    <t>Reese, M.</t>
+  </si>
+  <si>
+    <t>Reese Music</t>
+  </si>
+  <si>
+    <t>This is a test.</t>
   </si>
 </sst>
 </file>
@@ -433,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -461,22 +494,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -484,39 +517,39 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -581,36 +614,36 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
         <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
@@ -621,7 +654,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -630,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
@@ -641,22 +674,42 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>0</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add keyboard shortcuts
- All require combination with ALT
- ENTER = add, edit, save
- DELETE = delete
- H = help
- 1, 2, 3, 4 = four homeFrame selections
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
     <t>Sakura</t>
   </si>
@@ -27,6 +27,15 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>Iditarod</t>
+  </si>
+  <si>
+    <t>Soon Hee Newbold</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -71,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -79,21 +88,41 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>